<commit_message>
fixed part of mlp
</commit_message>
<xml_diff>
--- a/Cache/Metrics/Metrics.xlsx
+++ b/Cache/Metrics/Metrics.xlsx
@@ -541,11 +541,11 @@
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>39.38</v>
+        <v>39.59</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Wed Jun 12 17:26:49 2024</t>
+          <t>Thu Jun 13 08:47:43 2024</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,20 +671,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BernoulliNB(alpha=1)</t>
+          <t>RandomForestClassifier()</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7673821429084587</v>
+        <v>0.7683253588516746</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7543260963960052</v>
+        <v>0.8329550586191924</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01485837740238304</v>
+        <v>0.02435033385987805</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03754085420231147</v>
+        <v>0.0146266557147158</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -743,20 +743,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mean_classifier</t>
+          <t>KNeighborsClassifier(n_neighbors=20)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7673821429084587</v>
+        <v>0.6843992557150451</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7543260963960052</v>
+        <v>0.8484459883244077</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01485837740238304</v>
+        <v>0.03452429237957232</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03754085420231147</v>
+        <v>0.006929826070852984</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -797,6 +797,414 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AdaBoostClassifier(algorithm='SAMME', learning_rate=1)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.7622169059011165</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8409233125874463</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.02999158647670358</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.01289061083875735</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>HRV_Heart_rate</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>HRV_MeanNN</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>HRV_SDNN</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>700</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>WESAD</t>
+        </is>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DecisionTreeClassifier(max_depth=2)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.6477777777777778</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8119584599797366</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.03308113949591328</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.00583294529920401</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>HRV_Heart_rate</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>HRV_MeanNN</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>HRV_SDNN</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>700</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>WESAD</t>
+        </is>
+      </c>
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SVC()</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7574401913875597</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.8492543783470835</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.03557855856474591</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.01858333540622863</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>700</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>WESAD</t>
+        </is>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LinearDiscriminantAnalysis()</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.7442187163239795</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8365865055241954</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.04157821370232159</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.02094162707532396</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>HRV_Heart_rate</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>HRV_MeanNN</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>HRV_SDNN</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>700</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>WESAD</t>
+        </is>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BernoulliNB(alpha=1)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7673821429084587</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7543260963960052</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.01485837740238304</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.03754085420231147</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>HRV_Heart_rate</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>HRV_MeanNN</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>HRV_SDNN</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>700</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>WESAD</t>
+        </is>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mean_classifier</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.733108621266516</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8249213999682953</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.03056607169735969</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.01676369351534203</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>700</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>WESAD</t>
+        </is>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>